<commit_message>
Added Data to US Crime Rates by Region
</commit_message>
<xml_diff>
--- a/data/Crime_In_US_By_Region/Crime_In_US_By_Region_2018.xlsx
+++ b/data/Crime_In_US_By_Region/Crime_In_US_By_Region_2018.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4755FA5E-30C7-0743-93D6-B756DFAE6718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C542441B-1A50-C041-8F5B-32B8E0C66C84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18" x14ac:dyDescent="0.2"/>

</xml_diff>